<commit_message>
test(app): password hashing test
</commit_message>
<xml_diff>
--- a/doc/Cryptograph.xlsx
+++ b/doc/Cryptograph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22455" windowHeight="12195" activeTab="4"/>
+    <workbookView windowWidth="26430" windowHeight="11670" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Symetric" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="320">
   <si>
     <t>https://www.bouncycastle.org/specifications.html</t>
   </si>
@@ -1213,16 +1213,52 @@
   <si>
     <t>SHA512withECNR</t>
   </si>
+  <si>
+    <t>bcrypt</t>
+  </si>
+  <si>
+    <t>版本</t>
+  </si>
+  <si>
+    <t>cost factor 10</t>
+  </si>
+  <si>
+    <t>salt</t>
+  </si>
+  <si>
+    <t>salt len</t>
+  </si>
+  <si>
+    <t>迭代次数</t>
+  </si>
+  <si>
+    <t>加密串</t>
+  </si>
+  <si>
+    <t>scrypt</t>
+  </si>
+  <si>
+    <t>argon2</t>
+  </si>
+  <si>
+    <t>hash+salt</t>
+  </si>
+  <si>
+    <t>算法</t>
+  </si>
+  <si>
+    <t>pbkdf2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1280,7 +1316,98 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1294,106 +1421,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1409,7 +1438,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1436,7 +1472,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1448,13 +1604,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1466,7 +1616,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1478,127 +1634,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1616,7 +1652,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1660,26 +1696,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1701,9 +1737,44 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1722,41 +1793,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1765,10 +1801,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1777,19 +1813,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1798,112 +1834,112 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4364,14 +4400,88 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="B4:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="16.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:9">
+      <c r="B4" t="s">
+        <v>308</v>
+      </c>
+      <c r="D4" t="s">
+        <v>309</v>
+      </c>
+      <c r="E4" t="s">
+        <v>310</v>
+      </c>
+      <c r="F4" t="s">
+        <v>311</v>
+      </c>
+      <c r="G4" t="s">
+        <v>312</v>
+      </c>
+      <c r="H4" t="s">
+        <v>313</v>
+      </c>
+      <c r="I4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" t="s">
+        <v>317</v>
+      </c>
+      <c r="D7" t="s">
+        <v>318</v>
+      </c>
+      <c r="F7" t="s">
+        <v>311</v>
+      </c>
+      <c r="G7" t="s">
+        <v>312</v>
+      </c>
+      <c r="H7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" t="s">
+        <v>319</v>
+      </c>
+      <c r="D9" t="s">
+        <v>318</v>
+      </c>
+      <c r="F9" t="s">
+        <v>311</v>
+      </c>
+      <c r="G9" t="s">
+        <v>312</v>
+      </c>
+      <c r="H9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>